<commit_message>
Platform, Customer, and PSR in the excel.
</commit_message>
<xml_diff>
--- a/Output/DoD_Acq_Trends_OTA.xlsx
+++ b/Output/DoD_Acq_Trends_OTA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Users\Greg\Repositories\Vendor\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB53D449-1739-477B-A57D-1443C6BEBE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F98E8BC-3A41-4FBA-9A44-85A0FFC1D0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA790DA-767A-4A47-B819-9318ABA69B6C}"/>
   </bookViews>
@@ -10772,7 +10772,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17227,6 +17227,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010025DE50B441C283468F0A19FFD0E26C8A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aa546208bd87955cde426b286fb7c341">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f" xmlns:ns3="361d4f7d-a938-4275-8fcb-42d4143832a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ae09d569f748ab0a441a430c1e15f19" ns2:_="" ns3:_="">
     <xsd:import namespace="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f"/>
@@ -17463,12 +17469,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -17479,6 +17479,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3167479C-E6C8-488F-85AD-7849AC1912FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="361d4f7d-a938-4275-8fcb-42d4143832a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{379B5662-729B-45FF-B7E0-FF9D960BEDF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17497,23 +17514,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3167479C-E6C8-488F-85AD-7849AC1912FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="361d4f7d-a938-4275-8fcb-42d4143832a1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEC57303-5308-45F5-8961-50DD40D2FE8D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Front end of acq trends.
</commit_message>
<xml_diff>
--- a/Output/DoD_Acq_Trends_OTA.xlsx
+++ b/Output/DoD_Acq_Trends_OTA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Users\Greg\Repositories\Vendor\Output\"/>
     </mc:Choice>
@@ -30,7 +30,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="88">
   <si>
     <t>Row Labels</t>
   </si>
@@ -322,14 +322,17 @@
   <si>
     <t>OMB22_GDP20</t>
   </si>
+  <si>
+    <t>2022</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
@@ -455,7 +458,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -524,6 +527,123 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -10777,127 +10897,133 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="52.42578125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="20.42578125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.7109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="1">
-        <v>1000000000</v>
+      <c r="M1" s="60" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="47">
-        <v>393034568.82999998</v>
-      </c>
-      <c r="C2" s="47">
-        <v>474005596.36000001</v>
-      </c>
-      <c r="D2" s="47">
-        <v>340559772.73000002</v>
-      </c>
-      <c r="E2" s="47">
-        <v>523559084.60000002</v>
-      </c>
-      <c r="F2" s="47">
-        <v>695133317.67999995</v>
-      </c>
-      <c r="G2" s="47">
-        <v>1435155038.46</v>
-      </c>
-      <c r="H2" s="47">
-        <v>2126906395.3800001</v>
-      </c>
-      <c r="I2" s="47">
-        <v>4016160025.54</v>
-      </c>
-      <c r="J2" s="47">
-        <v>7458259913.9099998</v>
-      </c>
-      <c r="K2" s="47">
-        <v>16218548522.74</v>
-      </c>
-      <c r="L2" s="47">
-        <v>12159778208.280001</v>
+      <c r="B2" s="63" t="n">
+        <v>3.9303456883E8</v>
+      </c>
+      <c r="C2" s="65" t="n">
+        <v>4.7400559636E8</v>
+      </c>
+      <c r="D2" s="67" t="n">
+        <v>3.4055977273E8</v>
+      </c>
+      <c r="E2" s="69" t="n">
+        <v>5.235590846E8</v>
+      </c>
+      <c r="F2" s="71" t="n">
+        <v>6.9513331768E8</v>
+      </c>
+      <c r="G2" s="73" t="n">
+        <v>1.43515503846E9</v>
+      </c>
+      <c r="H2" s="75" t="n">
+        <v>2.12690639538E9</v>
+      </c>
+      <c r="I2" s="77" t="n">
+        <v>4.01651044854E9</v>
+      </c>
+      <c r="J2" s="79" t="n">
+        <v>7.46026433614E9</v>
+      </c>
+      <c r="K2" s="81" t="n">
+        <v>1.622187235366E10</v>
+      </c>
+      <c r="L2" s="83" t="n">
+        <v>1.536540327928E10</v>
+      </c>
+      <c r="M2" t="n" s="85">
+        <v>2.19201520844E9</v>
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="47">
-        <v>227972146.03</v>
-      </c>
-      <c r="C3" s="47">
-        <v>1115381865.6099999</v>
-      </c>
-      <c r="D3" s="47">
-        <v>273132033.56</v>
-      </c>
-      <c r="E3" s="47">
-        <v>4210858070.6500001</v>
-      </c>
-      <c r="F3" s="47">
-        <v>1748196128.04</v>
-      </c>
-      <c r="G3" s="47">
-        <v>11685154277.809999</v>
-      </c>
-      <c r="H3" s="47">
-        <v>11193300212.200001</v>
-      </c>
-      <c r="I3" s="47">
-        <v>27158765498.98</v>
-      </c>
-      <c r="J3" s="47">
-        <v>16574399713.26</v>
-      </c>
-      <c r="K3" s="47">
-        <v>17202822005.630001</v>
-      </c>
-      <c r="L3" s="47">
-        <v>61489894246.540001</v>
+      <c r="B3" s="64" t="n">
+        <v>2.2797214603E8</v>
+      </c>
+      <c r="C3" s="66" t="n">
+        <v>1.11538186561E9</v>
+      </c>
+      <c r="D3" s="68" t="n">
+        <v>2.7313203356E8</v>
+      </c>
+      <c r="E3" s="70" t="n">
+        <v>4.21085807065E9</v>
+      </c>
+      <c r="F3" s="72" t="n">
+        <v>1.74819612804E9</v>
+      </c>
+      <c r="G3" s="74" t="n">
+        <v>1.238515427781E10</v>
+      </c>
+      <c r="H3" s="76" t="n">
+        <v>1.11933002122E10</v>
+      </c>
+      <c r="I3" s="78" t="n">
+        <v>2.715947135598E10</v>
+      </c>
+      <c r="J3" s="80" t="n">
+        <v>1.659103374494E10</v>
+      </c>
+      <c r="K3" s="82" t="n">
+        <v>1.720503546323E10</v>
+      </c>
+      <c r="L3" s="84" t="n">
+        <v>6.7792073182409996E10</v>
+      </c>
+      <c r="M3" t="n" s="86">
+        <v>-8.8853536137E9</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -11042,10 +11168,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="19.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -11515,10 +11641,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="19.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -12058,13 +12184,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="8.25"/>
   <cols>
-    <col min="1" max="1" width="55.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="19"/>
-    <col min="10" max="10" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="19"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="19" width="55.140625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="19" width="12.140625" collapsed="false"/>
+    <col min="3" max="6" bestFit="true" customWidth="true" style="19" width="11.42578125" collapsed="false"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" style="19" width="12.140625" collapsed="false"/>
+    <col min="9" max="9" style="19" width="9.0" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="19" width="11.5703125" collapsed="false"/>
+    <col min="11" max="16384" style="19" width="9.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -13316,13 +13442,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="23" width="0" hidden="1" customWidth="1"/>
-    <col min="24" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="20" bestFit="1" customWidth="1"/>
-    <col min="29" max="34" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="38.0" collapsed="false"/>
+    <col min="2" max="23" customWidth="true" hidden="true" width="0.0" collapsed="false"/>
+    <col min="24" max="25" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
+    <col min="26" max="28" bestFit="true" customWidth="true" width="20.0" collapsed="false"/>
+    <col min="29" max="34" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="21.85546875" collapsed="false"/>
+    <col min="36" max="37" bestFit="true" customWidth="true" width="13.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -15301,8 +15427,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.0" collapsed="false"/>
+    <col min="14" max="19" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">

</xml_diff>

<commit_message>
Getting writing to excel working (key is the memory clear text)
</commit_message>
<xml_diff>
--- a/Output/DoD_Acq_Trends_OTA.xlsx
+++ b/Output/DoD_Acq_Trends_OTA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Users\Greg\Repositories\Vendor\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB53D449-1739-477B-A57D-1443C6BEBE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F4B750-927B-4DC7-8C15-534200BDE348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EA790DA-767A-4A47-B819-9318ABA69B6C}"/>
+    <workbookView xWindow="10305" yWindow="2190" windowWidth="16260" windowHeight="13485" activeTab="1" xr2:uid="{2EA790DA-767A-4A47-B819-9318ABA69B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Quarterly" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="88">
   <si>
     <t>Row Labels</t>
   </si>
@@ -331,8 +331,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
@@ -458,7 +458,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -524,9 +524,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4">
       <alignment wrapText="1"/>
     </xf>
@@ -578,70 +575,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10891,139 +10825,142 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415F8C06-381F-4E0B-AFB7-042671423187}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="52.42578125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="20.42578125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.7109375" collapsed="false"/>
+    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="56" t="s">
+      <c r="I1" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="58" t="s">
+      <c r="K1" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="M1" s="57" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="63" t="n">
-        <v>3.9303456883E8</v>
-      </c>
-      <c r="C2" s="65" t="n">
-        <v>4.7400559636E8</v>
-      </c>
-      <c r="D2" s="67" t="n">
-        <v>3.4055977273E8</v>
-      </c>
-      <c r="E2" s="69" t="n">
-        <v>5.235590846E8</v>
-      </c>
-      <c r="F2" s="71" t="n">
-        <v>6.9513331768E8</v>
-      </c>
-      <c r="G2" s="73" t="n">
-        <v>1.43515503846E9</v>
-      </c>
-      <c r="H2" s="75" t="n">
-        <v>2.12690639538E9</v>
-      </c>
-      <c r="I2" s="77" t="n">
-        <v>4.01651044854E9</v>
-      </c>
-      <c r="J2" s="79" t="n">
-        <v>7.46026433614E9</v>
-      </c>
-      <c r="K2" s="81" t="n">
-        <v>1.622187235366E10</v>
-      </c>
-      <c r="L2" s="83" t="n">
-        <v>1.536540327928E10</v>
-      </c>
-      <c r="M2" t="n" s="85">
-        <v>2.19201520844E9</v>
+      <c r="B2" s="62">
+        <v>393034568.82999998</v>
+      </c>
+      <c r="C2" s="62">
+        <v>474005596.36000001</v>
+      </c>
+      <c r="D2" s="62">
+        <v>340559772.73000002</v>
+      </c>
+      <c r="E2" s="62">
+        <v>523559084.60000002</v>
+      </c>
+      <c r="F2" s="62">
+        <v>695133317.67999995</v>
+      </c>
+      <c r="G2" s="62">
+        <v>1435155038.46</v>
+      </c>
+      <c r="H2" s="62">
+        <v>2126906395.3800001</v>
+      </c>
+      <c r="I2" s="62">
+        <v>4016510448.54</v>
+      </c>
+      <c r="J2" s="62">
+        <v>7460264336.1400003</v>
+      </c>
+      <c r="K2" s="62">
+        <v>16221872353.66</v>
+      </c>
+      <c r="L2" s="62">
+        <v>15365403279.280001</v>
+      </c>
+      <c r="M2" s="60">
+        <v>2192015208.4400001</v>
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="64" t="n">
-        <v>2.2797214603E8</v>
-      </c>
-      <c r="C3" s="66" t="n">
-        <v>1.11538186561E9</v>
-      </c>
-      <c r="D3" s="68" t="n">
-        <v>2.7313203356E8</v>
-      </c>
-      <c r="E3" s="70" t="n">
-        <v>4.21085807065E9</v>
-      </c>
-      <c r="F3" s="72" t="n">
-        <v>1.74819612804E9</v>
-      </c>
-      <c r="G3" s="74" t="n">
-        <v>1.238515427781E10</v>
-      </c>
-      <c r="H3" s="76" t="n">
-        <v>1.11933002122E10</v>
-      </c>
-      <c r="I3" s="78" t="n">
-        <v>2.715947135598E10</v>
-      </c>
-      <c r="J3" s="80" t="n">
-        <v>1.659103374494E10</v>
-      </c>
-      <c r="K3" s="82" t="n">
-        <v>1.720503546323E10</v>
-      </c>
-      <c r="L3" s="84" t="n">
-        <v>6.7792073182409996E10</v>
-      </c>
-      <c r="M3" t="n" s="86">
-        <v>-8.8853536137E9</v>
+      <c r="B3" s="62">
+        <v>227972146.03</v>
+      </c>
+      <c r="C3" s="62">
+        <v>1115381865.6099999</v>
+      </c>
+      <c r="D3" s="62">
+        <v>273132033.56</v>
+      </c>
+      <c r="E3" s="62">
+        <v>4210858070.6500001</v>
+      </c>
+      <c r="F3" s="62">
+        <v>1748196128.04</v>
+      </c>
+      <c r="G3" s="62">
+        <v>12385154277.809999</v>
+      </c>
+      <c r="H3" s="62">
+        <v>11193300212.200001</v>
+      </c>
+      <c r="I3" s="62">
+        <v>27159471355.98</v>
+      </c>
+      <c r="J3" s="62">
+        <v>16591033744.940001</v>
+      </c>
+      <c r="K3" s="62">
+        <v>17205035463.23</v>
+      </c>
+      <c r="L3" s="62">
+        <v>67792073182.409996</v>
+      </c>
+      <c r="M3" s="61">
+        <v>-8885353613.7000008</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -11168,10 +11105,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.28515625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="19.0" collapsed="false"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -11641,10 +11578,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.28515625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="19.0" collapsed="false"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -12184,13 +12121,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="8.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="19" width="55.140625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="19" width="12.140625" collapsed="false"/>
-    <col min="3" max="6" bestFit="true" customWidth="true" style="19" width="11.42578125" collapsed="false"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" style="19" width="12.140625" collapsed="false"/>
-    <col min="9" max="9" style="19" width="9.0" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="19" width="11.5703125" collapsed="false"/>
-    <col min="11" max="16384" style="19" width="9.0" collapsed="false"/>
+    <col min="1" max="1" width="55.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="19"/>
+    <col min="10" max="10" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -13442,13 +13379,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.0" collapsed="false"/>
-    <col min="2" max="23" customWidth="true" hidden="true" width="0.0" collapsed="false"/>
-    <col min="24" max="25" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="26" max="28" bestFit="true" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="29" max="34" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="36" max="37" bestFit="true" customWidth="true" width="13.5703125" collapsed="false"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="23" width="0" hidden="1" customWidth="1"/>
+    <col min="24" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="20" bestFit="1" customWidth="1"/>
+    <col min="29" max="34" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -15427,8 +15364,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.0" collapsed="false"/>
-    <col min="14" max="19" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="1" max="1" width="51" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -17353,6 +17290,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010025DE50B441C283468F0A19FFD0E26C8A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aa546208bd87955cde426b286fb7c341">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f" xmlns:ns3="361d4f7d-a938-4275-8fcb-42d4143832a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ae09d569f748ab0a441a430c1e15f19" ns2:_="" ns3:_="">
     <xsd:import namespace="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f"/>
@@ -17589,36 +17541,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{379B5662-729B-45FF-B7E0-FF9D960BEDF6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEC57303-5308-45F5-8961-50DD40D2FE8D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f"/>
-    <ds:schemaRef ds:uri="361d4f7d-a938-4275-8fcb-42d4143832a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17641,9 +17567,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEC57303-5308-45F5-8961-50DD40D2FE8D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{379B5662-729B-45FF-B7E0-FF9D960BEDF6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bec14128-4b25-4ac8-9cbb-ac2bd4640a4f"/>
+    <ds:schemaRef ds:uri="361d4f7d-a938-4275-8fcb-42d4143832a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>